<commit_message>
Started implementing comparison check
</commit_message>
<xml_diff>
--- a/Solution/Engine/AutoCorrector/Results.xlsx
+++ b/Solution/Engine/AutoCorrector/Results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -65,28 +65,37 @@
     <t>Yes</t>
   </si>
   <si>
-    <t xml:space="preserve"> fibonacci</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> There is no function provided to evaluate.</t>
+    <t>fibonacci</t>
+  </si>
+  <si>
+    <t>Input: 4 Expected Output: 3 Actual Output: 3Input: 5 Expected Output: 5 Actual Output: 5Success!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function respects the requirement because it has a single loop that iterates 'n' times, resulting in a time complexity of O(n).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function respects the requirement because it only uses a constant amount of space to store the variables fib, prevFib, and temp, which does not grow with the input size n, hence the space complexity is O(1) which is at most O(n).</t>
   </si>
   <si>
     <t>Input: 0 Expected Output: 0 Actual Output: 0Input: 1 Expected Output: 1 Actual Output: 1Success!</t>
   </si>
   <si>
+    <t xml:space="preserve"> The function does not handle incorrect input (negative numbers) as it does not check for negative values of n and will enter an infinite loop if n is negative.</t>
+  </si>
+  <si>
     <t>Alexe Robert George</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Please provide the requirement and the C++ function.</t>
+    <t>Input: 4 Expected Output: 3 Actual Output: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function's time complexity is not O(n) because the line "fib *= prevFib;" inside the loop causes the numbers to grow exponentially, leading to an exponential time complexity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function does not handle incorrect input (negative numbers and non-integers) as it does not include any error checking or handling for such cases.</t>
   </si>
   <si>
     <t>Alin Claudiu</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -145,15 +154,15 @@
     <col min="4" max="4" width="14.00644588470459" customWidth="1"/>
     <col min="5" max="5" width="12.145490646362305" customWidth="1"/>
     <col min="6" max="6" width="13.784440994262695" customWidth="1"/>
-    <col min="7" max="7" width="48.34665298461914" customWidth="1"/>
+    <col min="7" max="7" width="86.58473205566406" customWidth="1"/>
     <col min="8" max="8" width="13.784440994262695" customWidth="1"/>
-    <col min="9" max="9" width="48.34665298461914" customWidth="1"/>
+    <col min="9" max="9" width="156.9501190185547" customWidth="1"/>
     <col min="10" max="10" width="13.784440994262695" customWidth="1"/>
-    <col min="11" max="11" width="48.34665298461914" customWidth="1"/>
+    <col min="11" max="11" width="205.55699157714844" customWidth="1"/>
     <col min="12" max="12" width="13.784440994262695" customWidth="1"/>
     <col min="13" max="13" width="86.58473205566406" customWidth="1"/>
     <col min="14" max="14" width="13.784440994262695" customWidth="1"/>
-    <col min="15" max="15" width="48.34665298461914" customWidth="1"/>
+    <col min="15" max="15" width="136.68116760253906" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -208,7 +217,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="0">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>16</v>
@@ -217,75 +226,75 @@
         <v>17</v>
       </c>
       <c r="E2" s="0">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="0">
         <v>0.5</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N2" s="0">
         <v>0</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="0">
         <v>0</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="0">
         <v>0</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J3" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L3" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>21</v>
@@ -294,45 +303,45 @@
         <v>0</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J4" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M4" s="0" t="s">
         <v>21</v>
@@ -341,7 +350,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added highlight to signal similar code in source files
</commit_message>
<xml_diff>
--- a/Solution/Engine/AutoCorrector/Results.xlsx
+++ b/Solution/Engine/AutoCorrector/Results.xlsx
@@ -62,22 +62,22 @@
     <t>minPathLength</t>
   </si>
   <si>
+    <t xml:space="preserve"> The function respects the requirement. It correctly implements a BFS algorithm to find the shortest path between the start and end positions in the matrix, considering the given positions as obstacles. The function returns the minimum path length, which is 4 in this case, as expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function respects the requirement because it performs a BFS traversal of the matrix, which has a time complexity of O(n * m) in the worst case, and it also iterates over the given positions, which has a time complexity of O(k). Therefore, the overall time complexity is O(n * m + k), which is at most O(n * m * k) since k is less than or equal to n * m.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function respects the requirement because it uses a visited array of size n*m and a queue of maximum size n*m, resulting in a space complexity of O(n*m).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The function does not handle exceptions. There is no try-catch block or error checking mechanism to handle potential exceptions that may occur during the execution of the function.</t>
+  </si>
+  <si>
+    <t>Alexe Robert George</t>
+  </si>
+  <si>
     <t xml:space="preserve"> The function respects the requirement. It correctly implements a BFS algorithm to find the shortest path from the starting position to the ending position while avoiding the given positions. The function returns the minimum path length, which is 4 in this case, as expected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The function respects the requirement because it performs a BFS traversal of the matrix, which has a time complexity of O(n * m) in the worst case, and it also iterates through the given positions, which has a time complexity of O(k). Therefore, the overall time complexity is O(n * m + k), which is at most O(n * m * k) since k is less than or equal to n * m.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The function respects the requirement because it uses a visited array of size n*m and a queue to store the cells, which results in a space complexity of O(n*m).</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The function does not handle exceptions. There is no try-catch block or error checking mechanism to handle potential exceptions that may occur during the execution of the function.</t>
-  </si>
-  <si>
-    <t>Alexe Robert George</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The function respects the requirement. It correctly implements a BFS algorithm to find the shortest path between the starting and ending positions in the matrix, considering the given positions as obstacles. The function returns the minimum path length, which is 4 in this case, as expected.</t>
   </si>
   <si>
     <t xml:space="preserve"> The function respects the requirement because it performs a BFS traversal of the matrix, which has a time complexity of O(n*m) in the worst case, and it also iterates over the given positions, which has a time complexity of O(k). Therefore, the overall time complexity is O(n*m + k), which is at most O(n*m*k) since k is less than or equal to n*m.</t>
@@ -157,9 +157,9 @@
     <col min="4" max="4" width="14.044299125671387" customWidth="1"/>
     <col min="5" max="5" width="12.145490646362305" customWidth="1"/>
     <col min="6" max="6" width="13.784440994262695" customWidth="1"/>
-    <col min="7" max="7" width="254.80429077148438" customWidth="1"/>
+    <col min="7" max="7" width="249.51502990722656" customWidth="1"/>
     <col min="8" max="8" width="13.784440994262695" customWidth="1"/>
-    <col min="9" max="9" width="310.7158203125" customWidth="1"/>
+    <col min="9" max="9" width="307.6251525878906" customWidth="1"/>
     <col min="10" max="10" width="13.784440994262695" customWidth="1"/>
     <col min="11" max="11" width="160.44593811035156" customWidth="1"/>
     <col min="12" max="12" width="13.784440994262695" customWidth="1"/>

</xml_diff>

<commit_message>
Added possibility to save results into excel file after manually adjusting scores
</commit_message>
<xml_diff>
--- a/Solution/Engine/AutoCorrector/Results.xlsx
+++ b/Solution/Engine/AutoCorrector/Results.xlsx
@@ -212,7 +212,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="0">
-        <v>1.5</v>
+        <v>101</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
@@ -221,10 +221,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="0">
-        <v>1.5</v>
+        <v>101</v>
       </c>
       <c r="F2" s="0">
-        <v>0.5</v>
+        <v>100</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>16</v>

</xml_diff>